<commit_message>
add the ability to have more than one image for a material
</commit_message>
<xml_diff>
--- a/MaterialsWall/App_Data/data.xlsx
+++ b/MaterialsWall/App_Data/data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$157</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="500">
   <si>
     <t>PTFE (Teflon)</t>
   </si>
@@ -1531,6 +1531,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Has Primary Image</t>
+  </si>
+  <si>
+    <t>Has Secondary Image</t>
+  </si>
+  <si>
+    <t>Has Tertiary Image</t>
   </si>
 </sst>
 </file>
@@ -2013,13 +2022,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O157"/>
+  <dimension ref="A1:R157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B132" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A158" sqref="A158"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2027,14 +2036,17 @@
     <col min="1" max="1" width="54.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.90625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="5"/>
-    <col min="4" max="4" width="40.90625" style="5" customWidth="1"/>
-    <col min="5" max="8" width="28.90625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="35" style="3" customWidth="1"/>
-    <col min="10" max="15" width="21.6328125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.90625" style="5" customWidth="1"/>
+    <col min="8" max="11" width="28.90625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="35" style="3" customWidth="1"/>
+    <col min="13" max="18" width="21.6328125" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
@@ -2045,43 +2057,52 @@
         <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>251</v>
       </c>
@@ -2092,28 +2113,37 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2124,22 +2154,28 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2150,16 +2186,19 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>131</v>
       </c>
@@ -2170,16 +2209,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>278</v>
       </c>
@@ -2190,28 +2232,31 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
@@ -2222,16 +2267,19 @@
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -2242,16 +2290,19 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>125</v>
       </c>
@@ -2262,13 +2313,16 @@
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>120</v>
       </c>
@@ -2279,13 +2333,16 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>152</v>
       </c>
@@ -2296,13 +2353,16 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>153</v>
       </c>
@@ -2313,13 +2373,16 @@
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
@@ -2330,10 +2393,13 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>88</v>
       </c>
@@ -2344,13 +2410,16 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>88</v>
       </c>
@@ -2361,13 +2430,16 @@
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>197</v>
       </c>
@@ -2377,17 +2449,20 @@
       <c r="C16" s="5">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>104</v>
       </c>
@@ -2398,13 +2473,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -2415,13 +2493,16 @@
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>181</v>
       </c>
@@ -2432,19 +2513,22 @@
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>123</v>
       </c>
@@ -2455,13 +2539,16 @@
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>124</v>
       </c>
@@ -2472,13 +2559,16 @@
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>168</v>
       </c>
@@ -2489,16 +2579,19 @@
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2509,25 +2602,28 @@
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>122</v>
       </c>
@@ -2538,16 +2634,19 @@
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>167</v>
       </c>
@@ -2558,16 +2657,19 @@
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>151</v>
       </c>
@@ -2578,13 +2680,16 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
@@ -2595,13 +2700,16 @@
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>86</v>
       </c>
@@ -2612,13 +2720,16 @@
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>163</v>
       </c>
@@ -2629,16 +2740,19 @@
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>118</v>
       </c>
@@ -2649,13 +2763,16 @@
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>287</v>
       </c>
@@ -2666,23 +2783,26 @@
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="M31" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>246</v>
       </c>
@@ -2693,22 +2813,25 @@
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>140</v>
       </c>
@@ -2719,10 +2842,13 @@
         <v>33</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>105</v>
       </c>
@@ -2733,10 +2859,13 @@
         <v>34</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>165</v>
       </c>
@@ -2747,16 +2876,19 @@
         <v>35</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="L35" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
@@ -2767,10 +2899,13 @@
         <v>36</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>106</v>
       </c>
@@ -2781,10 +2916,13 @@
         <v>37</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>156</v>
       </c>
@@ -2795,16 +2933,19 @@
         <v>38</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="K38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="L38" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>285</v>
       </c>
@@ -2815,19 +2956,22 @@
         <v>39</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
@@ -2838,16 +2982,19 @@
         <v>40</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="K40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="L40" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>79</v>
       </c>
@@ -2857,17 +3004,20 @@
       <c r="C41" s="5">
         <v>41</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="K41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="L41" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>161</v>
       </c>
@@ -2878,10 +3028,13 @@
         <v>42</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>186</v>
       </c>
@@ -2892,19 +3045,22 @@
         <v>43</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="K43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="L43" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>84</v>
       </c>
@@ -2915,16 +3071,19 @@
         <v>44</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="J44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="K44" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -2935,13 +3094,16 @@
         <v>45</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="K45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>121</v>
       </c>
@@ -2952,13 +3114,16 @@
         <v>46</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="L46" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>169</v>
       </c>
@@ -2969,13 +3134,16 @@
         <v>47</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="K47" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>80</v>
       </c>
@@ -2986,22 +3154,25 @@
         <v>48</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="K48" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="L48" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>280</v>
       </c>
@@ -3012,19 +3183,22 @@
         <v>49</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>143</v>
       </c>
@@ -3035,10 +3209,13 @@
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>141</v>
       </c>
@@ -3049,10 +3226,13 @@
         <v>51</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>183</v>
       </c>
@@ -3063,13 +3243,16 @@
         <v>52</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="K52" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>162</v>
       </c>
@@ -3080,13 +3263,16 @@
         <v>53</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>144</v>
       </c>
@@ -3097,19 +3283,22 @@
         <v>54</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="K54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
@@ -3120,16 +3309,19 @@
         <v>55</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="J55" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="K55" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -3140,10 +3332,13 @@
         <v>56</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>30</v>
       </c>
@@ -3154,10 +3349,13 @@
         <v>57</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>288</v>
       </c>
@@ -3168,19 +3366,22 @@
         <v>58</v>
       </c>
       <c r="D58" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="J58" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="K58" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>187</v>
       </c>
@@ -3191,16 +3392,19 @@
         <v>59</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="J59" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="K59" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>171</v>
       </c>
@@ -3210,14 +3414,17 @@
       <c r="C60" s="5">
         <v>60</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="K60" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>289</v>
       </c>
@@ -3228,16 +3435,19 @@
         <v>61</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="K61" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>149</v>
       </c>
@@ -3248,13 +3458,16 @@
         <v>62</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="L62" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>90</v>
       </c>
@@ -3265,13 +3478,16 @@
         <v>63</v>
       </c>
       <c r="D63" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="L63" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>154</v>
       </c>
@@ -3282,16 +3498,19 @@
         <v>64</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G64" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="K64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="L64" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>185</v>
       </c>
@@ -3302,16 +3521,19 @@
         <v>65</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G65" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="J65" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="L65" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
@@ -3322,13 +3544,16 @@
         <v>66</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="K66" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>44</v>
       </c>
@@ -3339,16 +3564,19 @@
         <v>67</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="K67" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="L67" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>150</v>
       </c>
@@ -3359,19 +3587,22 @@
         <v>68</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="J68" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="K68" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="L68" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>203</v>
       </c>
@@ -3382,16 +3613,19 @@
         <v>69</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="K69" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>178</v>
       </c>
@@ -3402,19 +3636,22 @@
         <v>70</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G70" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="J70" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="K70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="L70" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>87</v>
       </c>
@@ -3425,13 +3662,16 @@
         <v>71</v>
       </c>
       <c r="D71" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G71" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="I71" s="3" t="s">
+      <c r="L71" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>132</v>
       </c>
@@ -3442,10 +3682,13 @@
         <v>72</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G72" s="5" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>283</v>
       </c>
@@ -3456,25 +3699,28 @@
         <v>73</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="J73" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="K73" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>159</v>
       </c>
@@ -3485,22 +3731,25 @@
         <v>74</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G74" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="K74" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="L74" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>166</v>
       </c>
@@ -3511,13 +3760,16 @@
         <v>75</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="K75" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>145</v>
       </c>
@@ -3528,22 +3780,25 @@
         <v>76</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="H76" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="I76" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="K76" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I76" s="3" t="s">
+      <c r="L76" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>158</v>
       </c>
@@ -3554,13 +3809,16 @@
         <v>77</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="I77" s="3" t="s">
+      <c r="L77" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>43</v>
       </c>
@@ -3571,10 +3829,13 @@
         <v>78</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>281</v>
       </c>
@@ -3585,22 +3846,25 @@
         <v>79</v>
       </c>
       <c r="D79" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G79" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="L79" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>49</v>
       </c>
@@ -3611,10 +3875,13 @@
         <v>80</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G80" s="5" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>116</v>
       </c>
@@ -3625,16 +3892,19 @@
         <v>81</v>
       </c>
       <c r="D81" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="K81" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J81" s="3" t="s">
+      <c r="M81" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>116</v>
       </c>
@@ -3645,13 +3915,16 @@
         <v>82</v>
       </c>
       <c r="D82" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G82" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="K82" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>109</v>
       </c>
@@ -3662,16 +3935,19 @@
         <v>83</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G83" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="I83" s="3" t="s">
+      <c r="L83" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="J83" s="3" t="s">
+      <c r="M83" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>2</v>
       </c>
@@ -3682,16 +3958,19 @@
         <v>84</v>
       </c>
       <c r="D84" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G84" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I84" s="3" t="s">
+      <c r="L84" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>117</v>
       </c>
@@ -3702,13 +3981,16 @@
         <v>85</v>
       </c>
       <c r="D85" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G85" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="L85" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>45</v>
       </c>
@@ -3719,10 +4001,13 @@
         <v>86</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G86" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
@@ -3733,16 +4018,19 @@
         <v>87</v>
       </c>
       <c r="D87" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G87" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="G87" s="3" t="s">
+      <c r="J87" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H87" s="3" t="s">
+      <c r="K87" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>75</v>
       </c>
@@ -3753,16 +4041,19 @@
         <v>88</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G88" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="G88" s="3" t="s">
+      <c r="J88" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="K88" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>98</v>
       </c>
@@ -3773,10 +4064,13 @@
         <v>89</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G89" s="5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>92</v>
       </c>
@@ -3787,19 +4081,22 @@
         <v>90</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G90" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="I90" s="3" t="s">
+      <c r="L90" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>85</v>
       </c>
@@ -3810,13 +4107,16 @@
         <v>91</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G91" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="I91" s="3" t="s">
+      <c r="L91" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -3827,16 +4127,19 @@
         <v>92</v>
       </c>
       <c r="D92" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G92" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="J92" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="L92" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>127</v>
       </c>
@@ -3847,16 +4150,19 @@
         <v>93</v>
       </c>
       <c r="D93" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="J93" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="L93" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>177</v>
       </c>
@@ -3867,19 +4173,22 @@
         <v>94</v>
       </c>
       <c r="D94" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G94" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="J94" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H94" s="3" t="s">
+      <c r="K94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="L94" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>290</v>
       </c>
@@ -3890,13 +4199,16 @@
         <v>95</v>
       </c>
       <c r="D95" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G95" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="L95" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>108</v>
       </c>
@@ -3907,10 +4219,13 @@
         <v>96</v>
       </c>
       <c r="D96" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G96" s="5" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>107</v>
       </c>
@@ -3921,10 +4236,13 @@
         <v>97</v>
       </c>
       <c r="D97" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G97" s="5" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>126</v>
       </c>
@@ -3934,14 +4252,17 @@
       <c r="C98" s="5">
         <v>98</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G98" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="I98" s="3" t="s">
+      <c r="L98" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>99</v>
       </c>
@@ -3952,10 +4273,13 @@
         <v>99</v>
       </c>
       <c r="D99" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G99" s="5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>99</v>
       </c>
@@ -3966,10 +4290,13 @@
         <v>100</v>
       </c>
       <c r="D100" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G100" s="5" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>130</v>
       </c>
@@ -3980,16 +4307,19 @@
         <v>101</v>
       </c>
       <c r="D101" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G101" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="J101" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="L101" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>91</v>
       </c>
@@ -4000,13 +4330,16 @@
         <v>102</v>
       </c>
       <c r="D102" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G102" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="I102" s="3" t="s">
+      <c r="L102" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>100</v>
       </c>
@@ -4017,19 +4350,22 @@
         <v>103</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G103" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="H103" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="K103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I103" s="3" t="s">
+      <c r="L103" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>202</v>
       </c>
@@ -4039,17 +4375,20 @@
       <c r="C104" s="5">
         <v>104</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D104" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G104" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="J104" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H104" s="3" t="s">
+      <c r="K104" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>205</v>
       </c>
@@ -4060,16 +4399,19 @@
         <v>105</v>
       </c>
       <c r="D105" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G105" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="G105" s="3" t="s">
+      <c r="J105" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="H105" s="3" t="s">
+      <c r="K105" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>0</v>
       </c>
@@ -4080,16 +4422,19 @@
         <v>106</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G106" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="H106" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="L106" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>213</v>
       </c>
@@ -4100,16 +4445,19 @@
         <v>107</v>
       </c>
       <c r="D107" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G107" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="H107" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="L107" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>129</v>
       </c>
@@ -4120,16 +4468,19 @@
         <v>108</v>
       </c>
       <c r="D108" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G108" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="H108" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I108" s="3" t="s">
+      <c r="L108" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>95</v>
       </c>
@@ -4140,16 +4491,19 @@
         <v>109</v>
       </c>
       <c r="D109" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G109" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="I109" s="3" t="s">
+      <c r="L109" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="J109" s="3" t="s">
+      <c r="M109" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>147</v>
       </c>
@@ -4160,13 +4514,16 @@
         <v>110</v>
       </c>
       <c r="D110" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G110" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="J110" s="3" t="s">
+      <c r="M110" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>31</v>
       </c>
@@ -4177,13 +4534,16 @@
         <v>111</v>
       </c>
       <c r="D111" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G111" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="H111" s="3" t="s">
+      <c r="K111" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>282</v>
       </c>
@@ -4194,22 +4554,25 @@
         <v>112</v>
       </c>
       <c r="D112" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G112" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="H112" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="L112" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="J112" s="3" t="s">
+      <c r="M112" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="L112" s="3" t="s">
+      <c r="O112" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>111</v>
       </c>
@@ -4220,13 +4583,16 @@
         <v>113</v>
       </c>
       <c r="D113" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G113" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="L113" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>82</v>
       </c>
@@ -4237,16 +4603,19 @@
         <v>114</v>
       </c>
       <c r="D114" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G114" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="J114" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H114" s="3" t="s">
+      <c r="K114" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>76</v>
       </c>
@@ -4257,16 +4626,19 @@
         <v>115</v>
       </c>
       <c r="D115" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G115" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="G115" s="3" t="s">
+      <c r="J115" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H115" s="3" t="s">
+      <c r="K115" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>128</v>
       </c>
@@ -4277,13 +4649,16 @@
         <v>116</v>
       </c>
       <c r="D116" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G116" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="I116" s="3" t="s">
+      <c r="L116" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>94</v>
       </c>
@@ -4294,13 +4669,16 @@
         <v>117</v>
       </c>
       <c r="D117" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G117" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="I117" s="3" t="s">
+      <c r="L117" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>47</v>
       </c>
@@ -4311,19 +4689,22 @@
         <v>118</v>
       </c>
       <c r="D118" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G118" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="H118" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H118" s="3" t="s">
+      <c r="K118" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I118" s="3" t="s">
+      <c r="L118" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>113</v>
       </c>
@@ -4334,13 +4715,16 @@
         <v>119</v>
       </c>
       <c r="D119" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G119" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="I119" s="3" t="s">
+      <c r="L119" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>160</v>
       </c>
@@ -4351,16 +4735,19 @@
         <v>120</v>
       </c>
       <c r="D120" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G120" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="H120" s="3" t="s">
+      <c r="K120" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I120" s="3" t="s">
+      <c r="L120" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>157</v>
       </c>
@@ -4371,16 +4758,19 @@
         <v>121</v>
       </c>
       <c r="D121" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G121" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="H121" s="3" t="s">
+      <c r="K121" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I121" s="3" t="s">
+      <c r="L121" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>157</v>
       </c>
@@ -4391,16 +4781,19 @@
         <v>122</v>
       </c>
       <c r="D122" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G122" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="H122" s="3" t="s">
+      <c r="K122" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I122" s="3" t="s">
+      <c r="L122" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>208</v>
       </c>
@@ -4411,16 +4804,19 @@
         <v>123</v>
       </c>
       <c r="D123" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G123" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="G123" s="3" t="s">
+      <c r="J123" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H123" s="3" t="s">
+      <c r="K123" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>284</v>
       </c>
@@ -4431,20 +4827,23 @@
         <v>124</v>
       </c>
       <c r="D124" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G124" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="H124" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="I124" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G124" s="2"/>
-      <c r="I124" s="2" t="s">
+      <c r="J124" s="2"/>
+      <c r="L124" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>112</v>
       </c>
@@ -4455,10 +4854,13 @@
         <v>125</v>
       </c>
       <c r="D125" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G125" s="5" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>33</v>
       </c>
@@ -4469,16 +4871,19 @@
         <v>126</v>
       </c>
       <c r="D126" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G126" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="G126" s="3" t="s">
+      <c r="J126" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I126" s="3" t="s">
+      <c r="L126" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>119</v>
       </c>
@@ -4489,13 +4894,16 @@
         <v>127</v>
       </c>
       <c r="D127" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G127" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="I127" s="3" t="s">
+      <c r="L127" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>114</v>
       </c>
@@ -4506,16 +4914,19 @@
         <v>128</v>
       </c>
       <c r="D128" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G128" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="I128" s="3" t="s">
+      <c r="L128" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="J128" s="3" t="s">
+      <c r="M128" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>194</v>
       </c>
@@ -4526,19 +4937,22 @@
         <v>129</v>
       </c>
       <c r="D129" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G129" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="E129" s="3" t="s">
+      <c r="H129" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H129" s="3" t="s">
+      <c r="K129" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I129" s="3" t="s">
+      <c r="L129" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>97</v>
       </c>
@@ -4549,19 +4963,22 @@
         <v>130</v>
       </c>
       <c r="D130" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G130" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="H130" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H130" s="3" t="s">
+      <c r="K130" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I130" s="3" t="s">
+      <c r="L130" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>29</v>
       </c>
@@ -4572,10 +4989,13 @@
         <v>131</v>
       </c>
       <c r="D131" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G131" s="5" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>32</v>
       </c>
@@ -4586,16 +5006,19 @@
         <v>132</v>
       </c>
       <c r="D132" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G132" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="H132" s="3" t="s">
+      <c r="K132" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I132" s="3" t="s">
+      <c r="L132" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>148</v>
       </c>
@@ -4606,19 +5029,22 @@
         <v>133</v>
       </c>
       <c r="D133" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G133" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="H133" s="3" t="s">
+      <c r="K133" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I133" s="3" t="s">
+      <c r="L133" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="J133" s="3" t="s">
+      <c r="M133" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>110</v>
       </c>
@@ -4629,13 +5055,16 @@
         <v>134</v>
       </c>
       <c r="D134" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G134" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="I134" s="2" t="s">
+      <c r="L134" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>103</v>
       </c>
@@ -4645,14 +5074,17 @@
       <c r="C135" s="5">
         <v>135</v>
       </c>
-      <c r="D135" s="7" t="s">
+      <c r="D135" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G135" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="I135" s="3" t="s">
+      <c r="L135" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>200</v>
       </c>
@@ -4663,13 +5095,16 @@
         <v>136</v>
       </c>
       <c r="D136" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G136" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="G136" s="3" t="s">
+      <c r="J136" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>73</v>
       </c>
@@ -4680,13 +5115,16 @@
         <v>137</v>
       </c>
       <c r="D137" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G137" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="G137" s="3" t="s">
+      <c r="J137" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>155</v>
       </c>
@@ -4697,16 +5135,19 @@
         <v>138</v>
       </c>
       <c r="D138" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G138" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="H138" s="3" t="s">
+      <c r="K138" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I138" s="3" t="s">
+      <c r="L138" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>133</v>
       </c>
@@ -4717,13 +5158,16 @@
         <v>139</v>
       </c>
       <c r="D139" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G139" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="I139" s="3" t="s">
+      <c r="L139" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>136</v>
       </c>
@@ -4734,10 +5178,13 @@
         <v>140</v>
       </c>
       <c r="D140" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G140" s="5" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>138</v>
       </c>
@@ -4748,10 +5195,13 @@
         <v>141</v>
       </c>
       <c r="D141" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G141" s="5" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>279</v>
       </c>
@@ -4762,22 +5212,25 @@
         <v>142</v>
       </c>
       <c r="D142" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G142" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="E142" s="2" t="s">
+      <c r="H142" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F142" s="2" t="s">
+      <c r="I142" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="I142" s="2" t="s">
+      <c r="L142" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="J142" s="3" t="s">
+      <c r="M142" s="3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>189</v>
       </c>
@@ -4788,16 +5241,19 @@
         <v>143</v>
       </c>
       <c r="D143" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G143" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="G143" s="3" t="s">
+      <c r="J143" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="H143" s="3" t="s">
+      <c r="K143" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>164</v>
       </c>
@@ -4808,13 +5264,16 @@
         <v>144</v>
       </c>
       <c r="D144" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G144" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="I144" s="3" t="s">
+      <c r="L144" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>176</v>
       </c>
@@ -4825,13 +5284,16 @@
         <v>145</v>
       </c>
       <c r="D145" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G145" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="I145" s="3" t="s">
+      <c r="L145" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>193</v>
       </c>
@@ -4842,10 +5304,13 @@
         <v>146</v>
       </c>
       <c r="D146" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G146" s="5" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>182</v>
       </c>
@@ -4856,16 +5321,19 @@
         <v>147</v>
       </c>
       <c r="D147" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G147" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="G147" s="3" t="s">
+      <c r="J147" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="H147" s="3" t="s">
+      <c r="K147" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>115</v>
       </c>
@@ -4876,13 +5344,16 @@
         <v>148</v>
       </c>
       <c r="D148" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G148" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="I148" s="2" t="s">
+      <c r="L148" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>139</v>
       </c>
@@ -4893,13 +5364,16 @@
         <v>149</v>
       </c>
       <c r="D149" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G149" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="I149" s="3" t="s">
+      <c r="L149" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>135</v>
       </c>
@@ -4910,10 +5384,13 @@
         <v>150</v>
       </c>
       <c r="D150" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G150" s="5" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>42</v>
       </c>
@@ -4924,10 +5401,13 @@
         <v>151</v>
       </c>
       <c r="D151" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G151" s="5" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>93</v>
       </c>
@@ -4938,16 +5418,19 @@
         <v>152</v>
       </c>
       <c r="D152" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G152" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="H152" s="3" t="s">
+      <c r="K152" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I152" s="3" t="s">
+      <c r="L152" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>134</v>
       </c>
@@ -4958,10 +5441,13 @@
         <v>153</v>
       </c>
       <c r="D153" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G153" s="5" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>291</v>
       </c>
@@ -4972,13 +5458,16 @@
         <v>154</v>
       </c>
       <c r="D154" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G154" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="I154" s="2" t="s">
+      <c r="L154" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>286</v>
       </c>
@@ -4989,28 +5478,31 @@
         <v>155</v>
       </c>
       <c r="D155" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G155" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E155" s="2" t="s">
+      <c r="H155" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F155" s="2" t="s">
+      <c r="I155" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G155" s="2" t="s">
+      <c r="J155" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="H155" s="3" t="s">
+      <c r="K155" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I155" s="2" t="s">
+      <c r="L155" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="J155" s="3" t="s">
+      <c r="M155" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>318</v>
       </c>
@@ -5021,13 +5513,16 @@
         <v>156</v>
       </c>
       <c r="D156" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G156" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="J156" s="3" t="s">
+      <c r="M156" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>319</v>
       </c>
@@ -5038,20 +5533,23 @@
         <v>157</v>
       </c>
       <c r="D157" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G157" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="J157" s="3" t="s">
+      <c r="M157" s="3" t="s">
         <v>320</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N157">
+  <autoFilter ref="A1:Q157">
     <sortState ref="A2:N157">
       <sortCondition ref="B1:B157"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J31" r:id="rId1"/>
+    <hyperlink ref="M31" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
remove the need to state how many images there are
</commit_message>
<xml_diff>
--- a/MaterialsWall/App_Data/data.xlsx
+++ b/MaterialsWall/App_Data/data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$157</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="497">
   <si>
     <t>PTFE (Teflon)</t>
   </si>
@@ -1531,15 +1531,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Has Primary Image</t>
-  </si>
-  <si>
-    <t>Has Secondary Image</t>
-  </si>
-  <si>
-    <t>Has Tertiary Image</t>
   </si>
 </sst>
 </file>
@@ -2022,13 +2013,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R157"/>
+  <dimension ref="A1:O157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2036,17 +2027,14 @@
     <col min="1" max="1" width="54.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.90625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="5"/>
-    <col min="4" max="4" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.90625" style="5" customWidth="1"/>
-    <col min="8" max="11" width="28.90625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="35" style="3" customWidth="1"/>
-    <col min="13" max="18" width="21.6328125" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="40.90625" style="5" customWidth="1"/>
+    <col min="5" max="8" width="28.90625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="35" style="3" customWidth="1"/>
+    <col min="10" max="15" width="21.6328125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
@@ -2057,52 +2045,43 @@
         <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>497</v>
+        <v>259</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>498</v>
+        <v>313</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>314</v>
+        <v>250</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>312</v>
+        <v>488</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>306</v>
+        <v>491</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>250</v>
+        <v>489</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>251</v>
       </c>
@@ -2113,37 +2092,28 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="L2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2154,28 +2124,22 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>334</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="I3" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="L3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2186,19 +2150,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G4" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>131</v>
       </c>
@@ -2209,19 +2170,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G5" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>278</v>
       </c>
@@ -2232,31 +2190,28 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G6" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="I6" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
@@ -2267,19 +2222,16 @@
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>210</v>
       </c>
@@ -2290,19 +2242,16 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>125</v>
       </c>
@@ -2313,16 +2262,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>120</v>
       </c>
@@ -2333,16 +2279,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>152</v>
       </c>
@@ -2353,16 +2296,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>153</v>
       </c>
@@ -2373,16 +2313,13 @@
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G12" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
@@ -2393,13 +2330,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" s="5" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>88</v>
       </c>
@@ -2410,16 +2344,13 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>88</v>
       </c>
@@ -2430,16 +2361,13 @@
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G15" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>197</v>
       </c>
@@ -2449,20 +2377,17 @@
       <c r="C16" s="5">
         <v>15</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>104</v>
       </c>
@@ -2473,16 +2398,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G17" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -2493,16 +2415,13 @@
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>181</v>
       </c>
@@ -2513,22 +2432,19 @@
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>123</v>
       </c>
@@ -2539,16 +2455,13 @@
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>124</v>
       </c>
@@ -2559,16 +2472,13 @@
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G21" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>168</v>
       </c>
@@ -2579,19 +2489,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2602,28 +2509,25 @@
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G23" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>122</v>
       </c>
@@ -2634,19 +2538,16 @@
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G24" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>167</v>
       </c>
@@ -2657,19 +2558,16 @@
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G25" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>151</v>
       </c>
@@ -2680,16 +2578,13 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G26" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
@@ -2700,16 +2595,13 @@
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G27" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>86</v>
       </c>
@@ -2720,16 +2612,13 @@
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G28" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>163</v>
       </c>
@@ -2740,19 +2629,16 @@
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G29" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>118</v>
       </c>
@@ -2763,16 +2649,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G30" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>287</v>
       </c>
@@ -2783,26 +2666,23 @@
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G31" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>342</v>
+      </c>
       <c r="I31" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="L31" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="J31" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>246</v>
       </c>
@@ -2813,25 +2693,22 @@
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G32" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>247</v>
       </c>
+      <c r="F32" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="I32" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="L32" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>140</v>
       </c>
@@ -2842,13 +2719,10 @@
         <v>33</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G33" s="5" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>105</v>
       </c>
@@ -2859,13 +2733,10 @@
         <v>34</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G34" s="5" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>165</v>
       </c>
@@ -2876,19 +2747,16 @@
         <v>35</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G35" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
@@ -2899,13 +2767,10 @@
         <v>36</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G36" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>106</v>
       </c>
@@ -2916,13 +2781,10 @@
         <v>37</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G37" s="5" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>156</v>
       </c>
@@ -2933,19 +2795,16 @@
         <v>38</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G38" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>285</v>
       </c>
@@ -2956,22 +2815,19 @@
         <v>39</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G39" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
@@ -2982,19 +2838,16 @@
         <v>40</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G40" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="I40" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>79</v>
       </c>
@@ -3004,20 +2857,17 @@
       <c r="C41" s="5">
         <v>41</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G41" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="I41" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>161</v>
       </c>
@@ -3028,13 +2878,10 @@
         <v>42</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G42" s="5" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>186</v>
       </c>
@@ -3045,22 +2892,19 @@
         <v>43</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G43" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="3" t="s">
+      <c r="I43" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>84</v>
       </c>
@@ -3071,19 +2915,16 @@
         <v>44</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G44" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -3094,16 +2935,13 @@
         <v>45</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G45" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>121</v>
       </c>
@@ -3114,16 +2952,13 @@
         <v>46</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G46" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="L46" s="3" t="s">
+      <c r="I46" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>169</v>
       </c>
@@ -3134,16 +2969,13 @@
         <v>47</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G47" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>80</v>
       </c>
@@ -3154,25 +2986,22 @@
         <v>48</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G48" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L48" s="3" t="s">
+      <c r="I48" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>280</v>
       </c>
@@ -3183,22 +3012,19 @@
         <v>49</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G49" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>241</v>
       </c>
+      <c r="F49" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="I49" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="L49" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>143</v>
       </c>
@@ -3209,13 +3035,10 @@
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G50" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>141</v>
       </c>
@@ -3226,13 +3049,10 @@
         <v>51</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G51" s="5" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>183</v>
       </c>
@@ -3243,16 +3063,13 @@
         <v>52</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G52" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>162</v>
       </c>
@@ -3263,16 +3080,13 @@
         <v>53</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G53" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>144</v>
       </c>
@@ -3283,22 +3097,19 @@
         <v>54</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G54" s="5" t="s">
         <v>395</v>
       </c>
+      <c r="E54" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="H54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L54" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
@@ -3309,19 +3120,16 @@
         <v>55</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G55" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -3332,13 +3140,10 @@
         <v>56</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G56" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>30</v>
       </c>
@@ -3349,13 +3154,10 @@
         <v>57</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G57" s="5" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>288</v>
       </c>
@@ -3366,22 +3168,19 @@
         <v>58</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G58" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="J58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K58" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>187</v>
       </c>
@@ -3392,19 +3191,16 @@
         <v>59</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G59" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="J59" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K59" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>171</v>
       </c>
@@ -3414,17 +3210,14 @@
       <c r="C60" s="5">
         <v>60</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G60" s="7" t="s">
+      <c r="D60" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>289</v>
       </c>
@@ -3435,19 +3228,16 @@
         <v>61</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G61" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="L61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>149</v>
       </c>
@@ -3458,16 +3248,13 @@
         <v>62</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G62" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="L62" s="3" t="s">
+      <c r="I62" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>90</v>
       </c>
@@ -3478,16 +3265,13 @@
         <v>63</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G63" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="L63" s="3" t="s">
+      <c r="I63" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>154</v>
       </c>
@@ -3498,19 +3282,16 @@
         <v>64</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G64" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="H64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L64" s="3" t="s">
+      <c r="I64" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>185</v>
       </c>
@@ -3521,19 +3302,16 @@
         <v>65</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G65" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="J65" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L65" s="3" t="s">
+      <c r="I65" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
@@ -3544,16 +3322,13 @@
         <v>66</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G66" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="K66" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>44</v>
       </c>
@@ -3564,19 +3339,16 @@
         <v>67</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G67" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="K67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="I67" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>150</v>
       </c>
@@ -3587,22 +3359,19 @@
         <v>68</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G68" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="J68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="H68" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="I68" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>203</v>
       </c>
@@ -3613,19 +3382,16 @@
         <v>69</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G69" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K69" s="3" t="s">
+      <c r="H69" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>178</v>
       </c>
@@ -3636,22 +3402,19 @@
         <v>70</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G70" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="J70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K70" s="3" t="s">
+      <c r="H70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L70" s="3" t="s">
+      <c r="I70" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>87</v>
       </c>
@@ -3662,16 +3425,13 @@
         <v>71</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G71" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="L71" s="3" t="s">
+      <c r="I71" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>132</v>
       </c>
@@ -3682,13 +3442,10 @@
         <v>72</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G72" s="5" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>283</v>
       </c>
@@ -3699,28 +3456,25 @@
         <v>73</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G73" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="I73" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L73" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>159</v>
       </c>
@@ -3731,25 +3485,22 @@
         <v>74</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G74" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="K74" s="3" t="s">
+      <c r="H74" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L74" s="3" t="s">
+      <c r="I74" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>166</v>
       </c>
@@ -3760,16 +3511,13 @@
         <v>75</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G75" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="K75" s="3" t="s">
+      <c r="H75" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>145</v>
       </c>
@@ -3780,25 +3528,22 @@
         <v>76</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G76" s="5" t="s">
         <v>414</v>
       </c>
+      <c r="E76" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="H76" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L76" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>158</v>
       </c>
@@ -3809,16 +3554,13 @@
         <v>77</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G77" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="L77" s="3" t="s">
+      <c r="I77" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>43</v>
       </c>
@@ -3829,13 +3571,10 @@
         <v>78</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G78" s="5" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>281</v>
       </c>
@@ -3846,25 +3585,22 @@
         <v>79</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G79" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>243</v>
       </c>
+      <c r="F79" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>245</v>
+      </c>
       <c r="I79" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="L79" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>49</v>
       </c>
@@ -3875,13 +3611,10 @@
         <v>80</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G80" s="5" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>116</v>
       </c>
@@ -3892,19 +3625,16 @@
         <v>81</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G81" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="K81" s="3" t="s">
+      <c r="H81" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M81" s="3" t="s">
+      <c r="J81" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>116</v>
       </c>
@@ -3915,16 +3645,13 @@
         <v>82</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G82" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="K82" s="3" t="s">
+      <c r="H82" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>109</v>
       </c>
@@ -3935,19 +3662,16 @@
         <v>83</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G83" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="L83" s="3" t="s">
+      <c r="I83" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="M83" s="3" t="s">
+      <c r="J83" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>2</v>
       </c>
@@ -3958,19 +3682,16 @@
         <v>84</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G84" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L84" s="3" t="s">
+      <c r="I84" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>117</v>
       </c>
@@ -3981,16 +3702,13 @@
         <v>85</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G85" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="L85" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>45</v>
       </c>
@@ -4001,13 +3719,10 @@
         <v>86</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G86" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
@@ -4018,19 +3733,16 @@
         <v>87</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G87" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="J87" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K87" s="3" t="s">
+      <c r="H87" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>75</v>
       </c>
@@ -4041,19 +3753,16 @@
         <v>88</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G88" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="J88" s="3" t="s">
+      <c r="G88" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K88" s="3" t="s">
+      <c r="H88" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>98</v>
       </c>
@@ -4064,13 +3773,10 @@
         <v>89</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G89" s="5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>92</v>
       </c>
@@ -4081,22 +3787,19 @@
         <v>90</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G90" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="L90" s="3" t="s">
+      <c r="I90" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>85</v>
       </c>
@@ -4107,16 +3810,13 @@
         <v>91</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G91" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="L91" s="3" t="s">
+      <c r="I91" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -4127,19 +3827,16 @@
         <v>92</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G92" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="J92" s="3" t="s">
+      <c r="G92" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L92" s="3" t="s">
+      <c r="I92" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>127</v>
       </c>
@@ -4150,19 +3847,16 @@
         <v>93</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G93" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="J93" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="L93" s="3" t="s">
+      <c r="I93" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>177</v>
       </c>
@@ -4173,22 +3867,19 @@
         <v>94</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G94" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="J94" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K94" s="3" t="s">
+      <c r="H94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L94" s="3" t="s">
+      <c r="I94" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>290</v>
       </c>
@@ -4199,16 +3890,13 @@
         <v>95</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G95" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="L95" s="2" t="s">
+      <c r="I95" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>108</v>
       </c>
@@ -4219,13 +3907,10 @@
         <v>96</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G96" s="5" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>107</v>
       </c>
@@ -4236,13 +3921,10 @@
         <v>97</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G97" s="5" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>126</v>
       </c>
@@ -4252,17 +3934,14 @@
       <c r="C98" s="5">
         <v>98</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G98" s="7" t="s">
+      <c r="D98" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="L98" s="3" t="s">
+      <c r="I98" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>99</v>
       </c>
@@ -4273,13 +3952,10 @@
         <v>99</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G99" s="5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>99</v>
       </c>
@@ -4290,13 +3966,10 @@
         <v>100</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G100" s="5" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>130</v>
       </c>
@@ -4307,19 +3980,16 @@
         <v>101</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G101" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="J101" s="3" t="s">
+      <c r="G101" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L101" s="3" t="s">
+      <c r="I101" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>91</v>
       </c>
@@ -4330,16 +4000,13 @@
         <v>102</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G102" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="L102" s="3" t="s">
+      <c r="I102" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>100</v>
       </c>
@@ -4350,22 +4017,19 @@
         <v>103</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G103" s="5" t="s">
         <v>438</v>
       </c>
+      <c r="E103" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H103" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L103" s="3" t="s">
+      <c r="I103" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>202</v>
       </c>
@@ -4375,20 +4039,17 @@
       <c r="C104" s="5">
         <v>104</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G104" s="7" t="s">
+      <c r="D104" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="J104" s="3" t="s">
+      <c r="G104" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="K104" s="3" t="s">
+      <c r="H104" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>205</v>
       </c>
@@ -4399,19 +4060,16 @@
         <v>105</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G105" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="J105" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="K105" s="3" t="s">
+      <c r="H105" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>0</v>
       </c>
@@ -4422,19 +4080,16 @@
         <v>106</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G106" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="H106" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L106" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>213</v>
       </c>
@@ -4445,19 +4100,16 @@
         <v>107</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G107" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="H107" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L107" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>129</v>
       </c>
@@ -4468,19 +4120,16 @@
         <v>108</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G108" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="H108" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L108" s="3" t="s">
+      <c r="I108" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>95</v>
       </c>
@@ -4491,19 +4140,16 @@
         <v>109</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G109" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="L109" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="M109" s="3" t="s">
+      <c r="J109" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>147</v>
       </c>
@@ -4514,16 +4160,13 @@
         <v>110</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G110" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="M110" s="3" t="s">
+      <c r="J110" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>31</v>
       </c>
@@ -4534,16 +4177,13 @@
         <v>111</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G111" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="K111" s="3" t="s">
+      <c r="H111" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>282</v>
       </c>
@@ -4554,25 +4194,22 @@
         <v>112</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G112" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="E112" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="L112" s="2" t="s">
+      <c r="I112" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="M112" s="3" t="s">
+      <c r="J112" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="O112" s="3" t="s">
+      <c r="L112" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>111</v>
       </c>
@@ -4583,16 +4220,13 @@
         <v>113</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G113" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="L113" s="3" t="s">
+      <c r="I113" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>82</v>
       </c>
@@ -4603,19 +4237,16 @@
         <v>114</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G114" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="J114" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K114" s="3" t="s">
+      <c r="H114" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>76</v>
       </c>
@@ -4626,19 +4257,16 @@
         <v>115</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G115" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="J115" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K115" s="3" t="s">
+      <c r="H115" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>128</v>
       </c>
@@ -4649,16 +4277,13 @@
         <v>116</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G116" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="L116" s="3" t="s">
+      <c r="I116" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>94</v>
       </c>
@@ -4669,16 +4294,13 @@
         <v>117</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G117" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="L117" s="3" t="s">
+      <c r="I117" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>47</v>
       </c>
@@ -4689,22 +4311,19 @@
         <v>118</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G118" s="5" t="s">
         <v>452</v>
       </c>
+      <c r="E118" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="H118" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K118" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L118" s="3" t="s">
+      <c r="I118" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>113</v>
       </c>
@@ -4715,16 +4334,13 @@
         <v>119</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G119" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="L119" s="3" t="s">
+      <c r="I119" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>160</v>
       </c>
@@ -4735,19 +4351,16 @@
         <v>120</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G120" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="K120" s="3" t="s">
+      <c r="H120" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L120" s="3" t="s">
+      <c r="I120" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>157</v>
       </c>
@@ -4758,19 +4371,16 @@
         <v>121</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G121" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="K121" s="3" t="s">
+      <c r="H121" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L121" s="3" t="s">
+      <c r="I121" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>157</v>
       </c>
@@ -4781,19 +4391,16 @@
         <v>122</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G122" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="K122" s="3" t="s">
+      <c r="H122" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L122" s="3" t="s">
+      <c r="I122" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>208</v>
       </c>
@@ -4804,19 +4411,16 @@
         <v>123</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G123" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="J123" s="3" t="s">
+      <c r="G123" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K123" s="3" t="s">
+      <c r="H123" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>284</v>
       </c>
@@ -4827,23 +4431,20 @@
         <v>124</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G124" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="E124" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="F124" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G124" s="2"/>
       <c r="I124" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J124" s="2"/>
-      <c r="L124" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>112</v>
       </c>
@@ -4854,13 +4455,10 @@
         <v>125</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G125" s="5" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>33</v>
       </c>
@@ -4871,19 +4469,16 @@
         <v>126</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G126" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="J126" s="3" t="s">
+      <c r="G126" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L126" s="3" t="s">
+      <c r="I126" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>119</v>
       </c>
@@ -4894,16 +4489,13 @@
         <v>127</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G127" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="L127" s="3" t="s">
+      <c r="I127" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>114</v>
       </c>
@@ -4914,19 +4506,16 @@
         <v>128</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G128" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="L128" s="3" t="s">
+      <c r="I128" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="M128" s="3" t="s">
+      <c r="J128" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>194</v>
       </c>
@@ -4937,22 +4526,19 @@
         <v>129</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G129" s="5" t="s">
         <v>462</v>
       </c>
+      <c r="E129" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="H129" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="K129" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L129" s="3" t="s">
+      <c r="I129" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>97</v>
       </c>
@@ -4963,22 +4549,19 @@
         <v>130</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G130" s="5" t="s">
         <v>463</v>
       </c>
+      <c r="E130" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H130" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K130" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L130" s="3" t="s">
+      <c r="I130" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>29</v>
       </c>
@@ -4989,13 +4572,10 @@
         <v>131</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G131" s="5" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>32</v>
       </c>
@@ -5006,19 +4586,16 @@
         <v>132</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G132" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="K132" s="3" t="s">
+      <c r="H132" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L132" s="3" t="s">
+      <c r="I132" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>148</v>
       </c>
@@ -5029,22 +4606,19 @@
         <v>133</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G133" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="K133" s="3" t="s">
+      <c r="H133" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L133" s="3" t="s">
+      <c r="I133" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="M133" s="3" t="s">
+      <c r="J133" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>110</v>
       </c>
@@ -5055,16 +4629,13 @@
         <v>134</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G134" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="L134" s="2" t="s">
+      <c r="I134" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>103</v>
       </c>
@@ -5074,17 +4645,14 @@
       <c r="C135" s="5">
         <v>135</v>
       </c>
-      <c r="D135" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G135" s="7" t="s">
+      <c r="D135" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="L135" s="3" t="s">
+      <c r="I135" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>200</v>
       </c>
@@ -5095,16 +4663,13 @@
         <v>136</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G136" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="J136" s="3" t="s">
+      <c r="G136" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>73</v>
       </c>
@@ -5115,16 +4680,13 @@
         <v>137</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G137" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="J137" s="3" t="s">
+      <c r="G137" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>155</v>
       </c>
@@ -5135,19 +4697,16 @@
         <v>138</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G138" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="K138" s="3" t="s">
+      <c r="H138" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L138" s="3" t="s">
+      <c r="I138" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>133</v>
       </c>
@@ -5158,16 +4717,13 @@
         <v>139</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G139" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="L139" s="3" t="s">
+      <c r="I139" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>136</v>
       </c>
@@ -5178,13 +4734,10 @@
         <v>140</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G140" s="5" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>138</v>
       </c>
@@ -5195,13 +4748,10 @@
         <v>141</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G141" s="5" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>279</v>
       </c>
@@ -5212,25 +4762,22 @@
         <v>142</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G142" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="H142" s="2" t="s">
+      <c r="E142" s="2" t="s">
         <v>257</v>
       </c>
+      <c r="F142" s="2" t="s">
+        <v>325</v>
+      </c>
       <c r="I142" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="L142" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="M142" s="3" t="s">
+      <c r="J142" s="3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>189</v>
       </c>
@@ -5241,19 +4788,16 @@
         <v>143</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G143" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="J143" s="3" t="s">
+      <c r="G143" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="K143" s="3" t="s">
+      <c r="H143" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>164</v>
       </c>
@@ -5264,16 +4808,13 @@
         <v>144</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G144" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="L144" s="3" t="s">
+      <c r="I144" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>176</v>
       </c>
@@ -5284,16 +4825,13 @@
         <v>145</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G145" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="L145" s="3" t="s">
+      <c r="I145" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>193</v>
       </c>
@@ -5304,13 +4842,10 @@
         <v>146</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G146" s="5" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>182</v>
       </c>
@@ -5321,19 +4856,16 @@
         <v>147</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G147" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="J147" s="3" t="s">
+      <c r="G147" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K147" s="3" t="s">
+      <c r="H147" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>115</v>
       </c>
@@ -5344,16 +4876,13 @@
         <v>148</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G148" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="L148" s="2" t="s">
+      <c r="I148" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>139</v>
       </c>
@@ -5364,16 +4893,13 @@
         <v>149</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G149" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="L149" s="3" t="s">
+      <c r="I149" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>135</v>
       </c>
@@ -5384,13 +4910,10 @@
         <v>150</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G150" s="5" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>42</v>
       </c>
@@ -5401,13 +4924,10 @@
         <v>151</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G151" s="5" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>93</v>
       </c>
@@ -5418,19 +4938,16 @@
         <v>152</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G152" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="K152" s="3" t="s">
+      <c r="H152" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L152" s="3" t="s">
+      <c r="I152" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>134</v>
       </c>
@@ -5441,13 +4958,10 @@
         <v>153</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G153" s="5" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>291</v>
       </c>
@@ -5458,16 +4972,13 @@
         <v>154</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G154" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="L154" s="2" t="s">
+      <c r="I154" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>286</v>
       </c>
@@ -5478,31 +4989,28 @@
         <v>155</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G155" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="H155" s="2" t="s">
+      <c r="E155" s="2" t="s">
         <v>258</v>
       </c>
+      <c r="F155" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="I155" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J155" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="K155" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L155" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="M155" s="3" t="s">
+      <c r="J155" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>318</v>
       </c>
@@ -5513,16 +5021,13 @@
         <v>156</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G156" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="M156" s="3" t="s">
+      <c r="J156" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>319</v>
       </c>
@@ -5533,23 +5038,20 @@
         <v>157</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G157" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="M157" s="3" t="s">
+      <c r="J157" s="3" t="s">
         <v>320</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q157">
+  <autoFilter ref="A1:N157">
     <sortState ref="A2:N157">
       <sortCondition ref="B1:B157"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="M31" r:id="rId1"/>
+    <hyperlink ref="J31" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>